<commit_message>
Added 7th, 8th and 10th grade questionssheet
</commit_message>
<xml_diff>
--- a/Documents/QuestionBank/7/7_BODMAS.xlsx
+++ b/Documents/QuestionBank/7/7_BODMAS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="559">
   <si>
     <t>No</t>
   </si>
@@ -1251,52 +1251,55 @@
     <t>3500</t>
   </si>
   <si>
+    <t>2650</t>
+  </si>
+  <si>
+    <t>3300</t>
+  </si>
+  <si>
+    <t>3400</t>
+  </si>
+  <si>
+    <t>First, calculate each component separately: \(200 \times 15 = 3000\); \(300 \div 2 = 150\); \(100 \times 5 = 500\). Then combine them: \((3000 + 150) - 500 = 2650\).</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>I_92</t>
+  </si>
+  <si>
+    <t>Evaluate \((5000 + 300 \times (450 - 200)) \div 250\).</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>320</t>
+  </si>
+  <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>First, evaluate the expression inside the brackets: \(450 - 200 = 250\). Then, multiply by 300: \(300 \times 250 = 75000\). Add 5000: \(5000 + 75000 = 80000\). Finally, divide by 250: \(\frac{80000}{250} = 320\).</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>I_93</t>
+  </si>
+  <si>
+    <t>Calculate \((60000 \div (300 - 175) + 1500) \times 4\).</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
     <t>3200</t>
-  </si>
-  <si>
-    <t>3300</t>
-  </si>
-  <si>
-    <t>3400</t>
-  </si>
-  <si>
-    <t>First, calculate each component separately: \(200 \times 15 = 3000\); \(300 \div 2 = 150\); \(100 \times 5 = 500\). Then combine them: \((3000 + 150) - 500 = 3200\).</t>
-  </si>
-  <si>
-    <t>92</t>
-  </si>
-  <si>
-    <t>I_92</t>
-  </si>
-  <si>
-    <t>Evaluate \((5000 + 300 \times (450 - 200)) \div 250\).</t>
-  </si>
-  <si>
-    <t>134</t>
-  </si>
-  <si>
-    <t>146</t>
-  </si>
-  <si>
-    <t>320</t>
-  </si>
-  <si>
-    <t>188</t>
-  </si>
-  <si>
-    <t>First, evaluate the expression inside the brackets: \(450 - 200 = 250\). Then, multiply by 300: \(300 \times 250 = 75000\). Add 5000: \(5000 + 75000 = 80000\). Finally, divide by 250: \(\frac{80000}{250} = 320\).</t>
-  </si>
-  <si>
-    <t>93</t>
-  </si>
-  <si>
-    <t>I_93</t>
-  </si>
-  <si>
-    <t>Calculate \((60000 \div (300 - 175) + 1500) \times 4\).</t>
-  </si>
-  <si>
-    <t>2000</t>
   </si>
   <si>
     <t>4000</t>
@@ -6029,13 +6032,13 @@
         <v>427</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>412</v>
+        <v>428</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="H98" s="6" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="I98" s="6" t="b">
         <v>1</v>
@@ -6047,7 +6050,7 @@
         <v>88</v>
       </c>
       <c r="L98" s="6" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="M98" s="6" t="s">
         <v>49</v>
@@ -6055,13 +6058,13 @@
     </row>
     <row r="99" ht="20.25" customHeight="1">
       <c r="A99" s="6" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>21</v>
@@ -6088,7 +6091,7 @@
         <v>26</v>
       </c>
       <c r="L99" s="6" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="M99" s="6" t="s">
         <v>49</v>
@@ -6096,28 +6099,28 @@
     </row>
     <row r="100" ht="20.25" customHeight="1">
       <c r="A100" s="6" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="H100" s="6" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="I100" s="6" t="b">
         <v>1</v>
@@ -6129,7 +6132,7 @@
         <v>26</v>
       </c>
       <c r="L100" s="6" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="M100" s="6" t="s">
         <v>49</v>
@@ -6138,16 +6141,16 @@
     <row r="101" ht="20.25" customHeight="1">
       <c r="A101" s="4"/>
       <c r="B101" s="5" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F101" s="4"/>
       <c r="G101" s="4"/>
@@ -6156,7 +6159,7 @@
         <v>1</v>
       </c>
       <c r="J101" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K101" s="4"/>
       <c r="L101" s="4"/>
@@ -6164,13 +6167,13 @@
     </row>
     <row r="102" ht="20.25" customHeight="1">
       <c r="A102" s="6" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>21</v>
@@ -6191,13 +6194,13 @@
         <v>1</v>
       </c>
       <c r="J102" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K102" s="6" t="s">
         <v>35</v>
       </c>
       <c r="L102" s="6" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="M102" s="6" t="s">
         <v>18</v>
@@ -6205,13 +6208,13 @@
     </row>
     <row r="103" ht="20.25" customHeight="1">
       <c r="A103" s="6" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>21</v>
@@ -6232,13 +6235,13 @@
         <v>1</v>
       </c>
       <c r="J103" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K103" s="6" t="s">
         <v>26</v>
       </c>
       <c r="L103" s="6" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M103" s="6" t="s">
         <v>18</v>
@@ -6249,10 +6252,10 @@
         <v>298</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>21</v>
@@ -6273,13 +6276,13 @@
         <v>1</v>
       </c>
       <c r="J104" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K104" s="6" t="s">
         <v>26</v>
       </c>
       <c r="L104" s="6" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="M104" s="6" t="s">
         <v>18</v>
@@ -6287,13 +6290,13 @@
     </row>
     <row r="105" ht="20.25" customHeight="1">
       <c r="A105" s="6" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>21</v>
@@ -6314,13 +6317,13 @@
         <v>1</v>
       </c>
       <c r="J105" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K105" s="6" t="s">
         <v>26</v>
       </c>
       <c r="L105" s="6" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="M105" s="6" t="s">
         <v>18</v>
@@ -6331,10 +6334,10 @@
         <v>78</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>21</v>
@@ -6355,13 +6358,13 @@
         <v>1</v>
       </c>
       <c r="J106" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K106" s="6" t="s">
         <v>95</v>
       </c>
       <c r="L106" s="6" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="M106" s="6" t="s">
         <v>18</v>
@@ -6369,13 +6372,13 @@
     </row>
     <row r="107" ht="20.25" customHeight="1">
       <c r="A107" s="6" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>21</v>
@@ -6396,13 +6399,13 @@
         <v>1</v>
       </c>
       <c r="J107" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K107" s="6" t="s">
         <v>35</v>
       </c>
       <c r="L107" s="6" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="M107" s="6" t="s">
         <v>28</v>
@@ -6410,13 +6413,13 @@
     </row>
     <row r="108" ht="20.25" customHeight="1">
       <c r="A108" s="6" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>21</v>
@@ -6437,13 +6440,13 @@
         <v>1</v>
       </c>
       <c r="J108" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K108" s="6" t="s">
         <v>95</v>
       </c>
       <c r="L108" s="6" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="M108" s="6" t="s">
         <v>28</v>
@@ -6451,13 +6454,13 @@
     </row>
     <row r="109" ht="20.25" customHeight="1">
       <c r="A109" s="6" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>21</v>
@@ -6478,13 +6481,13 @@
         <v>1</v>
       </c>
       <c r="J109" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K109" s="6" t="s">
         <v>95</v>
       </c>
       <c r="L109" s="6" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="M109" s="6" t="s">
         <v>28</v>
@@ -6492,13 +6495,13 @@
     </row>
     <row r="110" ht="20.25" customHeight="1">
       <c r="A110" s="6" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>21</v>
@@ -6519,13 +6522,13 @@
         <v>1</v>
       </c>
       <c r="J110" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K110" s="6" t="s">
         <v>88</v>
       </c>
       <c r="L110" s="6" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="M110" s="6" t="s">
         <v>28</v>
@@ -6533,13 +6536,13 @@
     </row>
     <row r="111" ht="20.25" customHeight="1">
       <c r="A111" s="6" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>21</v>
@@ -6560,13 +6563,13 @@
         <v>1</v>
       </c>
       <c r="J111" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K111" s="6" t="s">
         <v>88</v>
       </c>
       <c r="L111" s="6" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="M111" s="6" t="s">
         <v>28</v>
@@ -6574,13 +6577,13 @@
     </row>
     <row r="112" ht="20.25" customHeight="1">
       <c r="A112" s="6" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>21</v>
@@ -6601,13 +6604,13 @@
         <v>1</v>
       </c>
       <c r="J112" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K112" s="6" t="s">
         <v>26</v>
       </c>
       <c r="L112" s="6" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="M112" s="6" t="s">
         <v>37</v>
@@ -6615,13 +6618,13 @@
     </row>
     <row r="113" ht="20.25" customHeight="1">
       <c r="A113" s="6" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>21</v>
@@ -6642,13 +6645,13 @@
         <v>1</v>
       </c>
       <c r="J113" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K113" s="6" t="s">
         <v>35</v>
       </c>
       <c r="L113" s="6" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="M113" s="6" t="s">
         <v>37</v>
@@ -6656,13 +6659,13 @@
     </row>
     <row r="114" ht="20.25" customHeight="1">
       <c r="A114" s="6" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>21</v>
@@ -6683,13 +6686,13 @@
         <v>1</v>
       </c>
       <c r="J114" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K114" s="6" t="s">
         <v>35</v>
       </c>
       <c r="L114" s="6" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="M114" s="6" t="s">
         <v>37</v>
@@ -6697,13 +6700,13 @@
     </row>
     <row r="115" ht="20.25" customHeight="1">
       <c r="A115" s="6" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>21</v>
@@ -6724,13 +6727,13 @@
         <v>1</v>
       </c>
       <c r="J115" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K115" s="6" t="s">
         <v>26</v>
       </c>
       <c r="L115" s="6" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="M115" s="6" t="s">
         <v>37</v>
@@ -6738,13 +6741,13 @@
     </row>
     <row r="116" ht="20.25" customHeight="1">
       <c r="A116" s="6" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>21</v>
@@ -6765,13 +6768,13 @@
         <v>1</v>
       </c>
       <c r="J116" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K116" s="6" t="s">
         <v>26</v>
       </c>
       <c r="L116" s="6" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="M116" s="6" t="s">
         <v>37</v>
@@ -6779,13 +6782,13 @@
     </row>
     <row r="117" ht="20.25" customHeight="1">
       <c r="A117" s="6" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>21</v>
@@ -6806,13 +6809,13 @@
         <v>1</v>
       </c>
       <c r="J117" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K117" s="6" t="s">
         <v>95</v>
       </c>
       <c r="L117" s="6" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="M117" s="6" t="s">
         <v>44</v>
@@ -6820,13 +6823,13 @@
     </row>
     <row r="118" ht="20.25" customHeight="1">
       <c r="A118" s="6" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>21</v>
@@ -6847,13 +6850,13 @@
         <v>1</v>
       </c>
       <c r="J118" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K118" s="6" t="s">
         <v>95</v>
       </c>
       <c r="L118" s="6" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="M118" s="6" t="s">
         <v>44</v>
@@ -6861,40 +6864,40 @@
     </row>
     <row r="119" ht="20.25" customHeight="1">
       <c r="A119" s="6" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="H119" s="6" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="I119" s="6" t="b">
         <v>1</v>
       </c>
       <c r="J119" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K119" s="6" t="s">
         <v>26</v>
       </c>
       <c r="L119" s="6" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="M119" s="6" t="s">
         <v>44</v>
@@ -6902,13 +6905,13 @@
     </row>
     <row r="120" ht="20.25" customHeight="1">
       <c r="A120" s="6" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>21</v>
@@ -6929,13 +6932,13 @@
         <v>1</v>
       </c>
       <c r="J120" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K120" s="6" t="s">
         <v>26</v>
       </c>
       <c r="L120" s="6" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="M120" s="6" t="s">
         <v>44</v>
@@ -6943,13 +6946,13 @@
     </row>
     <row r="121" ht="20.25" customHeight="1">
       <c r="A121" s="6" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>21</v>
@@ -6970,13 +6973,13 @@
         <v>1</v>
       </c>
       <c r="J121" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K121" s="6" t="s">
         <v>35</v>
       </c>
       <c r="L121" s="6" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="M121" s="6" t="s">
         <v>44</v>
@@ -6984,13 +6987,13 @@
     </row>
     <row r="122" ht="20.25" customHeight="1">
       <c r="A122" s="6" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>21</v>
@@ -7005,19 +7008,19 @@
         <v>40</v>
       </c>
       <c r="H122" s="6" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="I122" s="6" t="b">
         <v>1</v>
       </c>
       <c r="J122" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K122" s="6" t="s">
         <v>88</v>
       </c>
       <c r="L122" s="6" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="M122" s="6" t="s">
         <v>49</v>
@@ -7025,13 +7028,13 @@
     </row>
     <row r="123" ht="20.25" customHeight="1">
       <c r="A123" s="6" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>21</v>
@@ -7052,13 +7055,13 @@
         <v>1</v>
       </c>
       <c r="J123" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K123" s="6" t="s">
         <v>26</v>
       </c>
       <c r="L123" s="6" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="M123" s="6" t="s">
         <v>49</v>
@@ -7066,13 +7069,13 @@
     </row>
     <row r="124" ht="20.25" customHeight="1">
       <c r="A124" s="6" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>21</v>
@@ -7093,13 +7096,13 @@
         <v>1</v>
       </c>
       <c r="J124" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K124" s="6" t="s">
         <v>26</v>
       </c>
       <c r="L124" s="6" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="M124" s="6" t="s">
         <v>49</v>
@@ -7107,13 +7110,13 @@
     </row>
     <row r="125" ht="20.25" customHeight="1">
       <c r="A125" s="6" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="D125" s="6" t="s">
         <v>21</v>
@@ -7134,13 +7137,13 @@
         <v>1</v>
       </c>
       <c r="J125" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K125" s="6" t="s">
         <v>26</v>
       </c>
       <c r="L125" s="6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M125" s="6" t="s">
         <v>49</v>
@@ -7148,13 +7151,13 @@
     </row>
     <row r="126" ht="20.25" customHeight="1">
       <c r="A126" s="6" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>21</v>
@@ -7175,13 +7178,13 @@
         <v>1</v>
       </c>
       <c r="J126" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K126" s="6" t="s">
         <v>95</v>
       </c>
       <c r="L126" s="6" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="M126" s="6" t="s">
         <v>49</v>
@@ -8078,27 +8081,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D2" s="10">
         <v>0.0</v>
@@ -8124,13 +8127,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="11" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="2">
@@ -8179,10 +8182,10 @@
     </row>
     <row r="6">
       <c r="A6" s="15" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C6" s="14" t="b">
         <v>1</v>

</xml_diff>